<commit_message>
Externalized start date and end date into assets
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S139958\Desktop\StockTicker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3A8EC2-5A50-4FF0-9BE2-ADEFE12DC4BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7755D63D-35A4-4566-A617-27125D109964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1440" windowWidth="27000" windowHeight="14235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>OutputPath</t>
-  </si>
-  <si>
-    <t>InputPDFFil</t>
   </si>
   <si>
     <t>Record</t>
@@ -278,6 +275,21 @@
 Filename processed er {{filename}}
 Mvh
 Stock Ticker Robot</t>
+  </si>
+  <si>
+    <t>InputMappe</t>
+  </si>
+  <si>
+    <t>Start_Dato</t>
+  </si>
+  <si>
+    <t>End_Dato</t>
+  </si>
+  <si>
+    <t>Start Date for Reporting. Format is dd-MM-yyyy</t>
+  </si>
+  <si>
+    <t>End Date for Reporting. Format is dd-MM-yyyy</t>
   </si>
 </sst>
 </file>
@@ -317,7 +329,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -343,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -354,6 +366,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1742,7 +1757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -1974,47 +1989,47 @@
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2995,10 +3010,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3053,13 +3068,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3067,7 +3082,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>53</v>
@@ -3078,47 +3093,67 @@
         <v>54</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>65</v>
-      </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="8">
+        <v>43447</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="8">
+        <v>43466</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4108,7 +4143,6 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://finance.yahoo.com/" xr:uid="{58222629-6A47-4BEE-87F7-61B54222FFC4}"/>

</xml_diff>